<commit_message>
MAR 10 - Edits on Mac
</commit_message>
<xml_diff>
--- a/notebooks/user_data/response_book.xlsx
+++ b/notebooks/user_data/response_book.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="user_list" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="user_00" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="user_list" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="user_00" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
@@ -704,10 +704,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D3" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1" s="5">
@@ -715,10 +715,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D4" s="4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1" s="5">

</xml_diff>

<commit_message>
MAR 12 EOD - After test w/ Richie
</commit_message>
<xml_diff>
--- a/notebooks/user_data/response_book.xlsx
+++ b/notebooks/user_data/response_book.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="user_list" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="user_00" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="user_list" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="user_00" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="user_01" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
@@ -457,11 +458,11 @@
   </sheetPr>
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="9.15" customWidth="1" style="3" min="1" max="1"/>
     <col width="26.9" customWidth="1" style="4" min="2" max="2"/>
@@ -495,6 +496,11 @@
       <c r="A3" s="3" t="inlineStr">
         <is>
           <t>01</t>
+        </is>
+      </c>
+      <c r="B3" s="4" t="inlineStr">
+        <is>
+          <t>richard attfield (beta test)</t>
         </is>
       </c>
     </row>
@@ -654,16 +660,16 @@
   </sheetPr>
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.15234375" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="9.4" customWidth="1" style="4" min="1" max="1"/>
     <col width="11.39" customWidth="1" style="4" min="2" max="2"/>
     <col width="12.05" customWidth="1" style="4" min="3" max="3"/>
-    <col width="16.9" customWidth="1" style="4" min="4" max="4"/>
+    <col width="16.89" customWidth="1" style="4" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1" s="5">
@@ -731,10 +737,10 @@
         <v>0</v>
       </c>
       <c r="C6" s="4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D6" s="4" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1" s="5">
@@ -753,10 +759,10 @@
         <v>2</v>
       </c>
       <c r="C8" s="4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D8" s="4" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1" s="5">
@@ -773,6 +779,196 @@
       </c>
       <c r="D10" s="4" t="n">
         <v>10</v>
+      </c>
+    </row>
+    <row r="11" ht="15" customHeight="1" s="5">
+      <c r="B11" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="4" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" ht="15" customHeight="1" s="5">
+      <c r="B12" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" s="4" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" ht="15" customHeight="1" s="5">
+      <c r="A14" s="4" t="inlineStr">
+        <is>
+          <t>sect3 libB</t>
+        </is>
+      </c>
+      <c r="B14" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="4" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" ht="15" customHeight="1" s="5">
+      <c r="B15" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="4" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" ht="15" customHeight="1" s="5">
+      <c r="B16" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" s="4" t="n">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup orientation="portrait" paperSize="1" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="0" useFirstPageNumber="0" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr filterMode="0">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetData>
+    <row r="1" ht="15" customHeight="1" s="5">
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Actual State</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Probed State</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>Probed Confidence</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15" customHeight="1" s="5">
+      <c r="A2" s="4" t="inlineStr">
+        <is>
+          <t>sect1 libA</t>
+        </is>
+      </c>
+      <c r="B2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" ht="15" customHeight="1" s="5">
+      <c r="B3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1" s="5">
+      <c r="B4" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" ht="15" customHeight="1" s="5">
+      <c r="A6" s="4" t="inlineStr">
+        <is>
+          <t>sect1 libB</t>
+        </is>
+      </c>
+      <c r="B6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" ht="15" customHeight="1" s="5">
+      <c r="B7" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" ht="15" customHeight="1" s="5">
+      <c r="B8" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" s="4" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" ht="15" customHeight="1" s="5">
+      <c r="A10" s="4" t="inlineStr">
+        <is>
+          <t>sect3 libA</t>
+        </is>
+      </c>
+      <c r="B10" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="4" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1" s="5">

</xml_diff>

<commit_message>
MAR 13 MID - Adding final save on matrix
</commit_message>
<xml_diff>
--- a/notebooks/user_data/response_book.xlsx
+++ b/notebooks/user_data/response_book.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t xml:space="preserve">user_ID</t>
   </si>
@@ -30,10 +30,16 @@
     <t xml:space="preserve">name</t>
   </si>
   <si>
+    <t xml:space="preserve">order</t>
+  </si>
+  <si>
     <t xml:space="preserve">00</t>
   </si>
   <si>
     <t xml:space="preserve">liam roy (beta test)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X – O</t>
   </si>
   <si>
     <t xml:space="preserve">01</t>
@@ -196,7 +202,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -206,6 +212,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -226,13 +236,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="26.9"/>
@@ -245,119 +255,131 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -382,7 +404,7 @@
       <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="9.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="11.39"/>
@@ -392,18 +414,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>0</v>
@@ -439,7 +461,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>0</v>
@@ -475,7 +497,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>0</v>
@@ -511,7 +533,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B14" s="2" t="n">
         <v>0</v>
@@ -571,18 +593,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="n">
         <v>0</v>
@@ -618,7 +640,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>0</v>
@@ -654,7 +676,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>0</v>
@@ -690,7 +712,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B14" s="2" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
MAR 15 - EOD with participant 17
</commit_message>
<xml_diff>
--- a/notebooks/user_data/response_book.xlsx
+++ b/notebooks/user_data/response_book.xlsx
@@ -20,6 +20,13 @@
     <sheet name="user_08" sheetId="10" state="visible" r:id="rId11"/>
     <sheet name="user_09" sheetId="11" state="visible" r:id="rId12"/>
     <sheet name="user_10" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="user_11" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="user_12" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="user_13" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="user_14" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="user_15" sheetId="17" state="visible" r:id="rId18"/>
+    <sheet name="user_16" sheetId="18" state="visible" r:id="rId19"/>
+    <sheet name="user_17" sheetId="19" state="visible" r:id="rId20"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -31,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="36">
   <si>
     <t xml:space="preserve">user_ID</t>
   </si>
@@ -63,7 +70,7 @@
     <t xml:space="preserve">03</t>
   </si>
   <si>
-    <t xml:space="preserve">real </t>
+    <t xml:space="preserve">done</t>
   </si>
   <si>
     <t xml:space="preserve">04</t>
@@ -232,7 +239,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -257,15 +264,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -349,7 +348,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H32" activeCellId="0" sqref="H32"/>
+      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -413,7 +412,7 @@
       <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="6" t="n">
+      <c r="D5" s="5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -427,7 +426,7 @@
       <c r="C6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="6" t="n">
+      <c r="D6" s="5" t="n">
         <v>2</v>
       </c>
     </row>
@@ -441,7 +440,7 @@
       <c r="C7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="6" t="n">
+      <c r="D7" s="5" t="n">
         <v>3</v>
       </c>
     </row>
@@ -455,7 +454,7 @@
       <c r="C8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="6" t="n">
+      <c r="D8" s="5" t="n">
         <v>4</v>
       </c>
     </row>
@@ -469,7 +468,7 @@
       <c r="C9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="6" t="n">
+      <c r="D9" s="5" t="n">
         <v>5</v>
       </c>
     </row>
@@ -483,7 +482,7 @@
       <c r="C10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="6" t="n">
+      <c r="D10" s="5" t="n">
         <v>6</v>
       </c>
     </row>
@@ -497,7 +496,7 @@
       <c r="C11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="6" t="n">
+      <c r="D11" s="5" t="n">
         <v>7</v>
       </c>
     </row>
@@ -511,7 +510,7 @@
       <c r="C12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="6" t="n">
+      <c r="D12" s="5" t="n">
         <v>8</v>
       </c>
     </row>
@@ -522,10 +521,10 @@
       <c r="B13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="8" t="n">
+      <c r="D13" s="6" t="n">
         <v>1</v>
       </c>
     </row>
@@ -533,8 +532,13 @@
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8" t="n">
+      <c r="B14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="6" t="n">
         <v>2</v>
       </c>
     </row>
@@ -542,8 +546,13 @@
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8" t="n">
+      <c r="B15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="6" t="n">
         <v>3</v>
       </c>
     </row>
@@ -551,8 +560,13 @@
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8" t="n">
+      <c r="B16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="6" t="n">
         <v>4</v>
       </c>
     </row>
@@ -560,8 +574,13 @@
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8" t="n">
+      <c r="B17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="6" t="n">
         <v>5</v>
       </c>
     </row>
@@ -569,8 +588,13 @@
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8" t="n">
+      <c r="B18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="6" t="n">
         <v>6</v>
       </c>
     </row>
@@ -578,8 +602,13 @@
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8" t="n">
+      <c r="B19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="6" t="n">
         <v>7</v>
       </c>
     </row>
@@ -587,8 +616,8 @@
       <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8" t="n">
+      <c r="C20" s="6"/>
+      <c r="D20" s="6" t="n">
         <v>8</v>
       </c>
     </row>
@@ -597,7 +626,7 @@
         <v>27</v>
       </c>
       <c r="C21" s="5"/>
-      <c r="D21" s="6" t="n">
+      <c r="D21" s="5" t="n">
         <v>9</v>
       </c>
     </row>
@@ -605,26 +634,26 @@
       <c r="A22" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="8" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C22" s="6"/>
+      <c r="D22" s="6" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
         <v>21</v>
       </c>
       <c r="C23" s="5"/>
-      <c r="D23" s="6" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D23" s="5" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="8" t="n">
+      <c r="C24" s="6"/>
+      <c r="D24" s="6" t="n">
         <v>10</v>
       </c>
     </row>
@@ -829,9 +858,9 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
         <v>29</v>
       </c>
@@ -842,7 +871,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>32</v>
       </c>
@@ -856,7 +885,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="2" t="n">
         <v>1</v>
       </c>
@@ -867,7 +896,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="2" t="n">
         <v>2</v>
       </c>
@@ -878,7 +907,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>33</v>
       </c>
@@ -892,7 +921,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="2" t="n">
         <v>1</v>
       </c>
@@ -903,7 +932,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="2" t="n">
         <v>2</v>
       </c>
@@ -914,7 +943,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
         <v>34</v>
       </c>
@@ -928,7 +957,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="2" t="n">
         <v>1</v>
       </c>
@@ -939,7 +968,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="2" t="n">
         <v>2</v>
       </c>
@@ -950,7 +979,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
         <v>35</v>
       </c>
@@ -964,7 +993,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="2" t="n">
         <v>1</v>
       </c>
@@ -975,7 +1004,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="2" t="n">
         <v>2</v>
       </c>
@@ -1008,6 +1037,1080 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B12" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B16" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B12" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B16" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B12" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B16" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B12" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B16" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B12" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B16" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q16" activeCellId="0" sqref="Q16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B12" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B16" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1032,7 +2135,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1040,10 +2143,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1054,7 +2157,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1068,7 +2171,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1076,10 +2179,10 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1087,10 +2190,10 @@
         <v>2</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1104,7 +2207,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1115,7 +2218,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1126,13 +2229,192 @@
         <v>2</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="B14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="B14" s="0" t="n">
         <v>0</v>
       </c>
@@ -1151,7 +2433,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1162,7 +2444,7 @@
         <v>2</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MAR 16 MID - After user 26 final
</commit_message>
<xml_diff>
--- a/notebooks/user_data/response_book.xlsx
+++ b/notebooks/user_data/response_book.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="27"/>
   </bookViews>
   <sheets>
     <sheet name="user_list" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,6 +27,15 @@
     <sheet name="user_15" sheetId="17" state="visible" r:id="rId18"/>
     <sheet name="user_16" sheetId="18" state="visible" r:id="rId19"/>
     <sheet name="user_17" sheetId="19" state="visible" r:id="rId20"/>
+    <sheet name="user_18" sheetId="20" state="visible" r:id="rId21"/>
+    <sheet name="user_19" sheetId="21" state="visible" r:id="rId22"/>
+    <sheet name="user_20" sheetId="22" state="visible" r:id="rId23"/>
+    <sheet name="user_21" sheetId="23" state="visible" r:id="rId24"/>
+    <sheet name="user_22" sheetId="24" state="visible" r:id="rId25"/>
+    <sheet name="user_23" sheetId="25" state="visible" r:id="rId26"/>
+    <sheet name="user_24" sheetId="26" state="visible" r:id="rId27"/>
+    <sheet name="user_25" sheetId="27" state="visible" r:id="rId28"/>
+    <sheet name="user_26" sheetId="28" state="visible" r:id="rId29"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -38,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="36">
   <si>
     <t xml:space="preserve">user_ID</t>
   </si>
@@ -345,10 +354,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -616,7 +625,12 @@
       <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="6"/>
+      <c r="B20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="D20" s="6" t="n">
         <v>8</v>
       </c>
@@ -625,8 +639,13 @@
       <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5" t="n">
+      <c r="B21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="6" t="n">
         <v>9</v>
       </c>
     </row>
@@ -634,27 +653,98 @@
       <c r="A22" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="6"/>
+      <c r="B22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="D22" s="6" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5" t="n">
-        <v>10</v>
+      <c r="B23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="6" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6" t="n">
-        <v>10</v>
+      <c r="B24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="5" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="5" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="5" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="5" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="6" t="n">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -2111,9 +2201,9 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
         <v>29</v>
       </c>
@@ -2124,7 +2214,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>32</v>
       </c>
@@ -2138,7 +2228,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="2" t="n">
         <v>1</v>
       </c>
@@ -2149,7 +2239,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="2" t="n">
         <v>2</v>
       </c>
@@ -2160,7 +2250,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>33</v>
       </c>
@@ -2174,7 +2264,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="2" t="n">
         <v>1</v>
       </c>
@@ -2185,7 +2275,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="2" t="n">
         <v>2</v>
       </c>
@@ -2196,7 +2286,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
         <v>34</v>
       </c>
@@ -2210,7 +2300,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="2" t="n">
         <v>1</v>
       </c>
@@ -2221,7 +2311,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="2" t="n">
         <v>2</v>
       </c>
@@ -2232,7 +2322,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
         <v>35</v>
       </c>
@@ -2246,7 +2336,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="2" t="n">
         <v>1</v>
       </c>
@@ -2257,7 +2347,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="2" t="n">
         <v>2</v>
       </c>
@@ -2290,9 +2380,9 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
         <v>29</v>
       </c>
@@ -2303,7 +2393,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>32</v>
       </c>
@@ -2317,7 +2407,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="2" t="n">
         <v>1</v>
       </c>
@@ -2328,7 +2418,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="2" t="n">
         <v>2</v>
       </c>
@@ -2339,7 +2429,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>33</v>
       </c>
@@ -2353,7 +2443,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="2" t="n">
         <v>1</v>
       </c>
@@ -2364,7 +2454,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="2" t="n">
         <v>2</v>
       </c>
@@ -2375,7 +2465,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
         <v>34</v>
       </c>
@@ -2389,7 +2479,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="2" t="n">
         <v>1</v>
       </c>
@@ -2400,7 +2490,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="2" t="n">
         <v>2</v>
       </c>
@@ -2411,39 +2501,39 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" s="0" t="n">
+      <c r="B14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="n">
         <v>4</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C15" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D15" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C16" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D16" s="0" t="n">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B16" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2" t="n">
         <v>7</v>
       </c>
     </row>
@@ -2643,6 +2733,1617 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B12" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B16" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B12" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B16" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B12" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B16" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B12" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B16" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B12" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B16" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B12" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B16" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B12" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B16" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B12" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B16" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R7" activeCellId="0" sqref="R7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">

</xml_diff>

<commit_message>
MAR 20 EOD - Finished plotter animation
</commit_message>
<xml_diff>
--- a/notebooks/user_data/response_book.xlsx
+++ b/notebooks/user_data/response_book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liamroy/Documents/Studies/Monash_31194990/PHD/repos/RL_audio/notebooks/user_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF2105C-AF80-724C-A49E-35A81FE40594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE650B84-8C6D-8C45-AB82-52CBF0DD761F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9482,10 +9482,10 @@
   <dimension ref="A1:BB38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="AG3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="AH3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AS21" sqref="AS21"/>
+      <selection pane="bottomRight" activeCell="AX20" sqref="AX20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
MAR 21 MID - Summed Matricies w/ vid
</commit_message>
<xml_diff>
--- a/notebooks/user_data/response_book.xlsx
+++ b/notebooks/user_data/response_book.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liamroy/Documents/Studies/Monash_31194990/PHD/repos/RL_audio/notebooks/user_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE650B84-8C6D-8C45-AB82-52CBF0DD761F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DE0E74D-35B5-8F41-9851-301D0EC6E662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="user_list" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
     <sheet name="user_25" sheetId="27" r:id="rId29"/>
     <sheet name="user_26" sheetId="28" r:id="rId30"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="108">
   <si>
     <t>user_ID</t>
   </si>
@@ -272,9 +272,6 @@
   </si>
   <si>
     <t>23</t>
-  </si>
-  <si>
-    <t>B</t>
   </si>
   <si>
     <t>TOTAL</t>
@@ -549,7 +546,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -764,11 +761,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -826,13 +832,13 @@
     <xf numFmtId="1" fontId="1" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -847,16 +853,7 @@
     <xf numFmtId="2" fontId="4" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -877,16 +874,13 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -949,55 +943,7 @@
     <xf numFmtId="2" fontId="4" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1009,18 +955,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1029,21 +963,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1054,38 +973,14 @@
     <xf numFmtId="2" fontId="4" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1141,10 +1036,64 @@
     <xf numFmtId="0" fontId="1" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1153,431 +1102,62 @@
     <xf numFmtId="0" fontId="1" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="45">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -7673,8 +7253,6 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:38" ht="18" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:38" ht="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>5</v>
@@ -9482,17 +9060,17 @@
   <dimension ref="A1:BB38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="AH3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AX20" sqref="AX20"/>
+      <selection pane="bottomRight" activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="15"/>
-    <col min="2" max="2" width="10.83203125" style="13"/>
-    <col min="3" max="3" width="14.83203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" style="15" customWidth="1"/>
+    <col min="2" max="2" width="12" style="13" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" style="13" customWidth="1"/>
     <col min="4" max="4" width="12" style="13" customWidth="1"/>
     <col min="5" max="5" width="11.83203125" style="13" bestFit="1" customWidth="1"/>
     <col min="6" max="41" width="12" style="13" customWidth="1"/>
@@ -9504,246 +9082,246 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:54" s="17" customFormat="1" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="107" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
+      <c r="D1" s="109" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" s="110"/>
+      <c r="F1" s="111" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="112"/>
+      <c r="H1" s="112"/>
+      <c r="I1" s="112"/>
+      <c r="J1" s="112"/>
+      <c r="K1" s="112"/>
+      <c r="L1" s="112"/>
+      <c r="M1" s="112"/>
+      <c r="N1" s="113"/>
+      <c r="O1" s="114" t="s">
+        <v>88</v>
+      </c>
+      <c r="P1" s="115"/>
+      <c r="Q1" s="115"/>
+      <c r="R1" s="115"/>
+      <c r="S1" s="115"/>
+      <c r="T1" s="115"/>
+      <c r="U1" s="115"/>
+      <c r="V1" s="115"/>
+      <c r="W1" s="116"/>
+      <c r="X1" s="117" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y1" s="118"/>
+      <c r="Z1" s="118"/>
+      <c r="AA1" s="118"/>
+      <c r="AB1" s="118"/>
+      <c r="AC1" s="118"/>
+      <c r="AD1" s="118"/>
+      <c r="AE1" s="118"/>
+      <c r="AF1" s="119"/>
+      <c r="AG1" s="120" t="s">
+        <v>90</v>
+      </c>
+      <c r="AH1" s="121"/>
+      <c r="AI1" s="121"/>
+      <c r="AJ1" s="121"/>
+      <c r="AK1" s="121"/>
+      <c r="AL1" s="121"/>
+      <c r="AM1" s="121"/>
+      <c r="AN1" s="121"/>
+      <c r="AO1" s="121"/>
+      <c r="AP1" s="89" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ1" s="90"/>
+      <c r="AR1" s="90"/>
+      <c r="AS1" s="90"/>
+      <c r="AT1" s="90"/>
+      <c r="AU1" s="91"/>
+      <c r="AV1" s="92" t="s">
+        <v>92</v>
+      </c>
+      <c r="AW1" s="93"/>
+      <c r="AX1" s="93"/>
+      <c r="AY1" s="93"/>
+      <c r="AZ1" s="93"/>
+      <c r="BA1" s="94"/>
+    </row>
+    <row r="2" spans="1:54" s="40" customFormat="1" ht="45" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="59" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="128" t="s">
-        <v>107</v>
-      </c>
-      <c r="E1" s="129"/>
-      <c r="F1" s="73" t="s">
+      <c r="C2" s="60" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="86" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="87" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-      <c r="L1" s="74"/>
-      <c r="M1" s="74"/>
-      <c r="N1" s="75"/>
-      <c r="O1" s="70" t="s">
-        <v>89</v>
-      </c>
-      <c r="P1" s="71"/>
-      <c r="Q1" s="71"/>
-      <c r="R1" s="71"/>
-      <c r="S1" s="71"/>
-      <c r="T1" s="71"/>
-      <c r="U1" s="71"/>
-      <c r="V1" s="71"/>
-      <c r="W1" s="72"/>
-      <c r="X1" s="67" t="s">
-        <v>90</v>
-      </c>
-      <c r="Y1" s="68"/>
-      <c r="Z1" s="68"/>
-      <c r="AA1" s="68"/>
-      <c r="AB1" s="68"/>
-      <c r="AC1" s="68"/>
-      <c r="AD1" s="68"/>
-      <c r="AE1" s="68"/>
-      <c r="AF1" s="69"/>
-      <c r="AG1" s="65" t="s">
-        <v>91</v>
-      </c>
-      <c r="AH1" s="66"/>
-      <c r="AI1" s="66"/>
-      <c r="AJ1" s="66"/>
-      <c r="AK1" s="66"/>
-      <c r="AL1" s="66"/>
-      <c r="AM1" s="66"/>
-      <c r="AN1" s="66"/>
-      <c r="AO1" s="66"/>
-      <c r="AP1" s="84" t="s">
-        <v>92</v>
-      </c>
-      <c r="AQ1" s="85"/>
-      <c r="AR1" s="85"/>
-      <c r="AS1" s="85"/>
-      <c r="AT1" s="85"/>
-      <c r="AU1" s="99"/>
-      <c r="AV1" s="76" t="s">
+      <c r="G2" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="J2" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="K2" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="L2" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="M2" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="N2" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="O2" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="P2" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q2" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="R2" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="S2" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="T2" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="U2" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="V2" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="W2" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="X2" s="54" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y2" s="48" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z2" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA2" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB2" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC2" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD2" s="47" t="s">
+        <v>86</v>
+      </c>
+      <c r="AE2" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="AF2" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG2" s="50" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH2" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI2" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ2" s="50" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK2" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL2" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="AM2" s="50" t="s">
+        <v>86</v>
+      </c>
+      <c r="AN2" s="51" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO2" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="AP2" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="AW1" s="77"/>
-      <c r="AX1" s="77"/>
-      <c r="AY1" s="77"/>
-      <c r="AZ1" s="77"/>
-      <c r="BA1" s="78"/>
-    </row>
-    <row r="2" spans="1:54" s="44" customFormat="1" ht="45" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
-        <v>80</v>
-      </c>
-      <c r="B2" s="79" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" s="80" t="s">
-        <v>81</v>
-      </c>
-      <c r="D2" s="123" t="s">
-        <v>62</v>
-      </c>
-      <c r="E2" s="124" t="s">
-        <v>63</v>
-      </c>
-      <c r="F2" s="45" t="s">
-        <v>83</v>
-      </c>
-      <c r="G2" s="46" t="s">
-        <v>84</v>
-      </c>
-      <c r="H2" s="47" t="s">
-        <v>61</v>
-      </c>
-      <c r="I2" s="45" t="s">
-        <v>85</v>
-      </c>
-      <c r="J2" s="46" t="s">
-        <v>86</v>
-      </c>
-      <c r="K2" s="47" t="s">
-        <v>61</v>
-      </c>
-      <c r="L2" s="45" t="s">
-        <v>87</v>
-      </c>
-      <c r="M2" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="N2" s="47" t="s">
-        <v>61</v>
-      </c>
-      <c r="O2" s="48" t="s">
-        <v>83</v>
-      </c>
-      <c r="P2" s="49" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q2" s="50" t="s">
-        <v>61</v>
-      </c>
-      <c r="R2" s="48" t="s">
-        <v>85</v>
-      </c>
-      <c r="S2" s="49" t="s">
-        <v>86</v>
-      </c>
-      <c r="T2" s="50" t="s">
-        <v>61</v>
-      </c>
-      <c r="U2" s="48" t="s">
-        <v>87</v>
-      </c>
-      <c r="V2" s="49" t="s">
-        <v>88</v>
-      </c>
-      <c r="W2" s="50" t="s">
-        <v>61</v>
-      </c>
-      <c r="X2" s="58" t="s">
-        <v>83</v>
-      </c>
-      <c r="Y2" s="52" t="s">
-        <v>84</v>
-      </c>
-      <c r="Z2" s="81" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA2" s="51" t="s">
-        <v>85</v>
-      </c>
-      <c r="AB2" s="52" t="s">
-        <v>86</v>
-      </c>
-      <c r="AC2" s="53" t="s">
-        <v>61</v>
-      </c>
-      <c r="AD2" s="51" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE2" s="52" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF2" s="53" t="s">
-        <v>61</v>
-      </c>
-      <c r="AG2" s="54" t="s">
-        <v>83</v>
-      </c>
-      <c r="AH2" s="55" t="s">
-        <v>84</v>
-      </c>
-      <c r="AI2" s="56" t="s">
-        <v>61</v>
-      </c>
-      <c r="AJ2" s="54" t="s">
-        <v>85</v>
-      </c>
-      <c r="AK2" s="55" t="s">
-        <v>86</v>
-      </c>
-      <c r="AL2" s="56" t="s">
-        <v>61</v>
-      </c>
-      <c r="AM2" s="54" t="s">
-        <v>87</v>
-      </c>
-      <c r="AN2" s="55" t="s">
-        <v>88</v>
-      </c>
-      <c r="AO2" s="56" t="s">
-        <v>61</v>
-      </c>
-      <c r="AP2" s="45" t="s">
+      <c r="AQ2" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="AQ2" s="57" t="s">
+      <c r="AR2" s="54" t="s">
         <v>95</v>
       </c>
-      <c r="AR2" s="58" t="s">
+      <c r="AS2" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="AS2" s="59" t="s">
+      <c r="AT2" s="62" t="s">
+        <v>72</v>
+      </c>
+      <c r="AU2" s="69" t="s">
+        <v>73</v>
+      </c>
+      <c r="AV2" s="41" t="s">
         <v>97</v>
       </c>
-      <c r="AT2" s="86" t="s">
-        <v>73</v>
-      </c>
-      <c r="AU2" s="100" t="s">
-        <v>74</v>
-      </c>
-      <c r="AV2" s="45" t="s">
+      <c r="AW2" s="53" t="s">
         <v>98</v>
       </c>
-      <c r="AW2" s="57" t="s">
+      <c r="AX2" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="AX2" s="58" t="s">
+      <c r="AY2" s="55" t="s">
         <v>100</v>
       </c>
-      <c r="AY2" s="59" t="s">
+      <c r="AZ2" s="63" t="s">
         <v>101</v>
       </c>
-      <c r="AZ2" s="87" t="s">
+      <c r="BA2" s="64" t="s">
         <v>102</v>
       </c>
-      <c r="BA2" s="88" t="s">
-        <v>103</v>
-      </c>
-      <c r="BB2" s="60"/>
+      <c r="BB2" s="56"/>
     </row>
     <row r="3" spans="1:54" x14ac:dyDescent="0.2">
-      <c r="A3" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="41" t="s">
+      <c r="A3" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="125" t="s">
+      <c r="C3" s="88" t="s">
         <v>37</v>
       </c>
       <c r="D3" s="18">
@@ -9806,7 +9384,7 @@
       <c r="W3" s="19">
         <v>9</v>
       </c>
-      <c r="X3" s="101">
+      <c r="X3" s="70">
         <v>0</v>
       </c>
       <c r="Y3" s="21">
@@ -9910,13 +9488,13 @@
       </c>
     </row>
     <row r="4" spans="1:54" x14ac:dyDescent="0.2">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="125" t="s">
+      <c r="B4" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="88" t="s">
         <v>37</v>
       </c>
       <c r="D4" s="18">
@@ -9979,7 +9557,7 @@
       <c r="W4" s="19">
         <v>5</v>
       </c>
-      <c r="X4" s="101">
+      <c r="X4" s="70">
         <v>0</v>
       </c>
       <c r="Y4" s="21">
@@ -10058,19 +9636,19 @@
         <v>2</v>
       </c>
       <c r="AV4" s="22">
-        <f t="shared" ref="AV4:AV27" si="6">AVERAGE(H4,K4,N4)</f>
+        <f t="shared" ref="AV4:AV26" si="6">AVERAGE(H4,K4,N4)</f>
         <v>5.666666666666667</v>
       </c>
       <c r="AW4" s="23">
-        <f t="shared" ref="AW4:AW27" si="7">AVERAGE(Q4,T4,W4)</f>
+        <f t="shared" ref="AW4:AW26" si="7">AVERAGE(Q4,T4,W4)</f>
         <v>6.333333333333333</v>
       </c>
       <c r="AX4" s="23">
-        <f t="shared" ref="AX4:AX27" si="8">AVERAGE(Z4,AC4,AF4)</f>
+        <f t="shared" ref="AX4:AX26" si="8">AVERAGE(Z4,AC4,AF4)</f>
         <v>9</v>
       </c>
       <c r="AY4" s="23">
-        <f t="shared" ref="AY4:AY27" si="9">AVERAGE(AI4,AL4,AO4)</f>
+        <f t="shared" ref="AY4:AY26" si="9">AVERAGE(AI4,AL4,AO4)</f>
         <v>8.3333333333333339</v>
       </c>
       <c r="AZ4" s="23">
@@ -10083,13 +9661,13 @@
       </c>
     </row>
     <row r="5" spans="1:54" x14ac:dyDescent="0.2">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="125" t="s">
+      <c r="B5" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="88" t="s">
         <v>37</v>
       </c>
       <c r="D5" s="18">
@@ -10152,7 +9730,7 @@
       <c r="W5" s="19">
         <v>6</v>
       </c>
-      <c r="X5" s="101">
+      <c r="X5" s="70">
         <v>0</v>
       </c>
       <c r="Y5" s="21">
@@ -10256,13 +9834,13 @@
       </c>
     </row>
     <row r="6" spans="1:54" x14ac:dyDescent="0.2">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="125" t="s">
+      <c r="C6" s="88" t="s">
         <v>37</v>
       </c>
       <c r="D6" s="18">
@@ -10325,7 +9903,7 @@
       <c r="W6" s="19">
         <v>4</v>
       </c>
-      <c r="X6" s="101">
+      <c r="X6" s="70">
         <v>0</v>
       </c>
       <c r="Y6" s="21">
@@ -10429,13 +10007,13 @@
       </c>
     </row>
     <row r="7" spans="1:54" x14ac:dyDescent="0.2">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="125" t="s">
+      <c r="C7" s="88" t="s">
         <v>37</v>
       </c>
       <c r="D7" s="18">
@@ -10498,7 +10076,7 @@
       <c r="W7" s="19">
         <v>10</v>
       </c>
-      <c r="X7" s="101">
+      <c r="X7" s="70">
         <v>0</v>
       </c>
       <c r="Y7" s="21">
@@ -10602,13 +10180,13 @@
       </c>
     </row>
     <row r="8" spans="1:54" x14ac:dyDescent="0.2">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="125" t="s">
+      <c r="C8" s="88" t="s">
         <v>37</v>
       </c>
       <c r="D8" s="18">
@@ -10671,7 +10249,7 @@
       <c r="W8" s="19">
         <v>9</v>
       </c>
-      <c r="X8" s="101">
+      <c r="X8" s="70">
         <v>0</v>
       </c>
       <c r="Y8" s="21">
@@ -10775,13 +10353,13 @@
       </c>
     </row>
     <row r="9" spans="1:54" x14ac:dyDescent="0.2">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="125" t="s">
+      <c r="C9" s="88" t="s">
         <v>37</v>
       </c>
       <c r="D9" s="18">
@@ -10844,7 +10422,7 @@
       <c r="W9" s="19">
         <v>8</v>
       </c>
-      <c r="X9" s="101">
+      <c r="X9" s="70">
         <v>0</v>
       </c>
       <c r="Y9" s="21">
@@ -10948,13 +10526,13 @@
       </c>
     </row>
     <row r="10" spans="1:54" x14ac:dyDescent="0.2">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="125" t="s">
+      <c r="C10" s="88" t="s">
         <v>37</v>
       </c>
       <c r="D10" s="18">
@@ -11017,7 +10595,7 @@
       <c r="W10" s="19">
         <v>4</v>
       </c>
-      <c r="X10" s="101">
+      <c r="X10" s="70">
         <v>0</v>
       </c>
       <c r="Y10" s="21">
@@ -11121,13 +10699,13 @@
       </c>
     </row>
     <row r="11" spans="1:54" x14ac:dyDescent="0.2">
-      <c r="A11" s="40">
+      <c r="A11" s="36">
         <v>22</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="125" t="s">
+      <c r="C11" s="88" t="s">
         <v>37</v>
       </c>
       <c r="D11" s="18">
@@ -11190,7 +10768,7 @@
       <c r="W11" s="19">
         <v>8</v>
       </c>
-      <c r="X11" s="101">
+      <c r="X11" s="70">
         <v>0</v>
       </c>
       <c r="Y11" s="21">
@@ -11294,13 +10872,13 @@
       </c>
     </row>
     <row r="12" spans="1:54" x14ac:dyDescent="0.2">
-      <c r="A12" s="40">
+      <c r="A12" s="36">
         <v>23</v>
       </c>
-      <c r="B12" s="41" t="s">
+      <c r="B12" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="125" t="s">
+      <c r="C12" s="88" t="s">
         <v>37</v>
       </c>
       <c r="D12" s="18">
@@ -11363,7 +10941,7 @@
       <c r="W12" s="19">
         <v>7</v>
       </c>
-      <c r="X12" s="101">
+      <c r="X12" s="70">
         <v>0</v>
       </c>
       <c r="Y12" s="21">
@@ -11467,13 +11045,13 @@
       </c>
     </row>
     <row r="13" spans="1:54" x14ac:dyDescent="0.2">
-      <c r="A13" s="40">
+      <c r="A13" s="36">
         <v>24</v>
       </c>
-      <c r="B13" s="41" t="s">
+      <c r="B13" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="125" t="s">
+      <c r="C13" s="88" t="s">
         <v>37</v>
       </c>
       <c r="D13" s="18">
@@ -11536,7 +11114,7 @@
       <c r="W13" s="19">
         <v>9</v>
       </c>
-      <c r="X13" s="101">
+      <c r="X13" s="70">
         <v>0</v>
       </c>
       <c r="Y13" s="21">
@@ -11640,13 +11218,13 @@
       </c>
     </row>
     <row r="14" spans="1:54" x14ac:dyDescent="0.2">
-      <c r="A14" s="40">
+      <c r="A14" s="36">
         <v>25</v>
       </c>
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="125" t="s">
+      <c r="C14" s="88" t="s">
         <v>37</v>
       </c>
       <c r="D14" s="18">
@@ -11709,7 +11287,7 @@
       <c r="W14" s="19">
         <v>8</v>
       </c>
-      <c r="X14" s="101">
+      <c r="X14" s="70">
         <v>0</v>
       </c>
       <c r="Y14" s="21">
@@ -11813,13 +11391,13 @@
       </c>
     </row>
     <row r="15" spans="1:54" x14ac:dyDescent="0.2">
-      <c r="A15" s="40" t="s">
+      <c r="A15" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="41" t="s">
+      <c r="B15" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="42" t="s">
+      <c r="C15" s="38" t="s">
         <v>38</v>
       </c>
       <c r="D15" s="18">
@@ -11882,7 +11460,7 @@
       <c r="W15" s="19">
         <v>8</v>
       </c>
-      <c r="X15" s="101">
+      <c r="X15" s="70">
         <v>0</v>
       </c>
       <c r="Y15" s="21">
@@ -11986,13 +11564,13 @@
       </c>
     </row>
     <row r="16" spans="1:54" x14ac:dyDescent="0.2">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="42" t="s">
+      <c r="C16" s="38" t="s">
         <v>38</v>
       </c>
       <c r="D16" s="18">
@@ -12055,7 +11633,7 @@
       <c r="W16" s="19">
         <v>5</v>
       </c>
-      <c r="X16" s="101">
+      <c r="X16" s="70">
         <v>0</v>
       </c>
       <c r="Y16" s="21">
@@ -12159,13 +11737,13 @@
       </c>
     </row>
     <row r="17" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="42" t="s">
+      <c r="C17" s="38" t="s">
         <v>38</v>
       </c>
       <c r="D17" s="18">
@@ -12228,7 +11806,7 @@
       <c r="W17" s="19">
         <v>5</v>
       </c>
-      <c r="X17" s="101">
+      <c r="X17" s="70">
         <v>0</v>
       </c>
       <c r="Y17" s="21">
@@ -12332,13 +11910,13 @@
       </c>
     </row>
     <row r="18" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A18" s="40" t="s">
+      <c r="A18" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="42" t="s">
+      <c r="C18" s="38" t="s">
         <v>38</v>
       </c>
       <c r="D18" s="18">
@@ -12401,7 +11979,7 @@
       <c r="W18" s="19">
         <v>2</v>
       </c>
-      <c r="X18" s="101">
+      <c r="X18" s="70">
         <v>0</v>
       </c>
       <c r="Y18" s="21">
@@ -12505,13 +12083,13 @@
       </c>
     </row>
     <row r="19" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="41" t="s">
+      <c r="B19" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="42" t="s">
+      <c r="C19" s="38" t="s">
         <v>38</v>
       </c>
       <c r="D19" s="18">
@@ -12574,7 +12152,7 @@
       <c r="W19" s="19">
         <v>7</v>
       </c>
-      <c r="X19" s="101">
+      <c r="X19" s="70">
         <v>0</v>
       </c>
       <c r="Y19" s="21">
@@ -12678,13 +12256,13 @@
       </c>
     </row>
     <row r="20" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A20" s="40" t="s">
+      <c r="A20" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="41" t="s">
+      <c r="B20" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="38" t="s">
         <v>38</v>
       </c>
       <c r="D20" s="18">
@@ -12747,7 +12325,7 @@
       <c r="W20" s="19">
         <v>10</v>
       </c>
-      <c r="X20" s="101">
+      <c r="X20" s="70">
         <v>0</v>
       </c>
       <c r="Y20" s="21">
@@ -12851,13 +12429,13 @@
       </c>
     </row>
     <row r="21" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A21" s="40" t="s">
+      <c r="A21" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="41" t="s">
+      <c r="B21" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="42" t="s">
+      <c r="C21" s="38" t="s">
         <v>38</v>
       </c>
       <c r="D21" s="18">
@@ -12920,7 +12498,7 @@
       <c r="W21" s="19">
         <v>4</v>
       </c>
-      <c r="X21" s="101">
+      <c r="X21" s="70">
         <v>0</v>
       </c>
       <c r="Y21" s="21">
@@ -13024,13 +12602,13 @@
       </c>
     </row>
     <row r="22" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A22" s="40" t="s">
+      <c r="A22" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="41" t="s">
+      <c r="B22" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="42" t="s">
+      <c r="C22" s="38" t="s">
         <v>38</v>
       </c>
       <c r="D22" s="18">
@@ -13093,7 +12671,7 @@
       <c r="W22" s="19">
         <v>8</v>
       </c>
-      <c r="X22" s="101">
+      <c r="X22" s="70">
         <v>0</v>
       </c>
       <c r="Y22" s="21">
@@ -13197,13 +12775,13 @@
       </c>
     </row>
     <row r="23" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A23" s="40" t="s">
+      <c r="A23" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="41" t="s">
+      <c r="B23" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="42" t="s">
+      <c r="C23" s="38" t="s">
         <v>38</v>
       </c>
       <c r="D23" s="18">
@@ -13266,7 +12844,7 @@
       <c r="W23" s="19">
         <v>4</v>
       </c>
-      <c r="X23" s="101">
+      <c r="X23" s="70">
         <v>0</v>
       </c>
       <c r="Y23" s="21">
@@ -13370,13 +12948,13 @@
       </c>
     </row>
     <row r="24" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A24" s="40" t="s">
+      <c r="A24" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="41" t="s">
+      <c r="B24" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="C24" s="42" t="s">
+      <c r="C24" s="38" t="s">
         <v>38</v>
       </c>
       <c r="D24" s="18">
@@ -13439,7 +13017,7 @@
       <c r="W24" s="19">
         <v>5</v>
       </c>
-      <c r="X24" s="101">
+      <c r="X24" s="70">
         <v>0</v>
       </c>
       <c r="Y24" s="21">
@@ -13543,13 +13121,13 @@
       </c>
     </row>
     <row r="25" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A25" s="40">
+      <c r="A25" s="36">
         <v>21</v>
       </c>
-      <c r="B25" s="41" t="s">
+      <c r="B25" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="42" t="s">
+      <c r="C25" s="38" t="s">
         <v>38</v>
       </c>
       <c r="D25" s="18">
@@ -13612,7 +13190,7 @@
       <c r="W25" s="19">
         <v>6</v>
       </c>
-      <c r="X25" s="101">
+      <c r="X25" s="70">
         <v>0</v>
       </c>
       <c r="Y25" s="21">
@@ -13716,13 +13294,13 @@
       </c>
     </row>
     <row r="26" spans="1:53" ht="22" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="40">
+      <c r="A26" s="36">
         <v>26</v>
       </c>
-      <c r="B26" s="41" t="s">
-        <v>108</v>
-      </c>
-      <c r="C26" s="42" t="s">
+      <c r="B26" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="C26" s="38" t="s">
         <v>38</v>
       </c>
       <c r="D26" s="18">
@@ -13785,7 +13363,7 @@
       <c r="W26" s="19">
         <v>9</v>
       </c>
-      <c r="X26" s="101">
+      <c r="X26" s="70">
         <v>0</v>
       </c>
       <c r="Y26" s="21">
@@ -13888,502 +13466,502 @@
         <v>0.66666666666666607</v>
       </c>
     </row>
-    <row r="27" spans="1:53" s="34" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="B27" s="89"/>
-      <c r="C27" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="D27" s="37">
+    <row r="27" spans="1:53" s="31" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="95" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" s="96"/>
+      <c r="C27" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="34">
         <f>SUM(D3:D26)</f>
         <v>964</v>
       </c>
-      <c r="E27" s="34">
+      <c r="E27" s="31">
         <f>SUM(E3:E26)</f>
         <v>402</v>
       </c>
-      <c r="F27" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="G27" s="34">
+      <c r="F27" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="G27" s="31">
         <f>COUNTIF(G3:G26, "=0")</f>
         <v>21</v>
       </c>
-      <c r="H27" s="39"/>
-      <c r="I27" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="J27" s="34">
+      <c r="H27" s="35"/>
+      <c r="I27" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="J27" s="31">
         <f>COUNTIF(J3:J26, "=1")</f>
         <v>11</v>
       </c>
-      <c r="K27" s="39"/>
-      <c r="L27" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="M27" s="34">
+      <c r="K27" s="35"/>
+      <c r="L27" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="M27" s="31">
         <f>COUNTIF(M3:M26, "=2")</f>
         <v>14</v>
       </c>
-      <c r="N27" s="39"/>
-      <c r="O27" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="P27" s="34">
+      <c r="N27" s="35"/>
+      <c r="O27" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="P27" s="31">
         <f>COUNTIF(P3:P26, "=0")</f>
         <v>20</v>
       </c>
-      <c r="Q27" s="39"/>
-      <c r="R27" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="S27" s="34">
+      <c r="Q27" s="35"/>
+      <c r="R27" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="S27" s="31">
         <f>COUNTIF(S3:S26, "=1")</f>
         <v>16</v>
       </c>
-      <c r="T27" s="39"/>
-      <c r="U27" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="V27" s="34">
+      <c r="T27" s="35"/>
+      <c r="U27" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="V27" s="31">
         <f>COUNTIF(V3:V26, "=2")</f>
         <v>16</v>
       </c>
-      <c r="W27" s="39"/>
-      <c r="X27" s="61" t="s">
-        <v>71</v>
-      </c>
-      <c r="Y27" s="34">
+      <c r="W27" s="35"/>
+      <c r="X27" s="57" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y27" s="31">
         <f>COUNTIF(Y3:Y26, "=0")</f>
         <v>22</v>
       </c>
-      <c r="Z27" s="35"/>
-      <c r="AA27" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="AB27" s="34">
+      <c r="Z27" s="32"/>
+      <c r="AA27" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB27" s="31">
         <f>COUNTIF(AB3:AB26, "=1")</f>
         <v>23</v>
       </c>
-      <c r="AC27" s="39"/>
-      <c r="AD27" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="AE27" s="34">
+      <c r="AC27" s="35"/>
+      <c r="AD27" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE27" s="31">
         <f>COUNTIF(AE3:AE26, "=2")</f>
         <v>21</v>
       </c>
-      <c r="AF27" s="39"/>
-      <c r="AG27" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="AH27" s="34">
+      <c r="AF27" s="35"/>
+      <c r="AG27" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH27" s="31">
         <f>COUNTIF(AH3:AH26, "=0")</f>
         <v>21</v>
       </c>
-      <c r="AI27" s="39"/>
-      <c r="AJ27" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="AK27" s="34">
+      <c r="AI27" s="35"/>
+      <c r="AJ27" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="AK27" s="31">
         <f>COUNTIF(AK3:AK26, "=1")</f>
         <v>20</v>
       </c>
-      <c r="AL27" s="39"/>
-      <c r="AM27" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="AN27" s="34">
+      <c r="AL27" s="35"/>
+      <c r="AM27" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN27" s="31">
         <f>COUNTIF(AN3:AN26, "=2")</f>
         <v>24</v>
       </c>
-      <c r="AO27" s="39"/>
-      <c r="AP27" s="63">
+      <c r="AO27" s="35"/>
+      <c r="AP27" s="34">
         <f>SUM(AP3:AP26)</f>
         <v>46</v>
       </c>
-      <c r="AQ27" s="38">
+      <c r="AQ27" s="31">
         <f>SUM(AQ3:AQ26)</f>
         <v>52</v>
       </c>
-      <c r="AR27" s="38">
+      <c r="AR27" s="31">
         <f>SUM(AR3:AR26)</f>
         <v>66</v>
       </c>
-      <c r="AS27" s="38">
+      <c r="AS27" s="31">
         <f>SUM(AS3:AS26)</f>
         <v>65</v>
       </c>
-      <c r="AT27" s="119">
+      <c r="AT27" s="82">
         <f t="shared" si="4"/>
         <v>20</v>
       </c>
-      <c r="AU27" s="120">
+      <c r="AU27" s="83">
         <f t="shared" si="5"/>
         <v>13</v>
       </c>
-      <c r="AV27" s="64"/>
-      <c r="AW27" s="35"/>
-      <c r="AX27" s="35"/>
-      <c r="AY27" s="35"/>
-      <c r="AZ27" s="35"/>
-      <c r="BA27" s="39"/>
-    </row>
-    <row r="28" spans="1:53" s="34" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="90"/>
-      <c r="B28" s="91"/>
-      <c r="C28" s="94" t="s">
-        <v>104</v>
-      </c>
-      <c r="D28" s="117">
+      <c r="AV27" s="58"/>
+      <c r="AW27" s="32"/>
+      <c r="AX27" s="32"/>
+      <c r="AY27" s="32"/>
+      <c r="AZ27" s="32"/>
+      <c r="BA27" s="35"/>
+    </row>
+    <row r="28" spans="1:53" s="31" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="97"/>
+      <c r="B28" s="98"/>
+      <c r="C28" s="65" t="s">
+        <v>103</v>
+      </c>
+      <c r="D28" s="80">
         <f>AVERAGE(D3:D26)</f>
         <v>40.166666666666664</v>
       </c>
-      <c r="E28" s="118">
+      <c r="E28" s="81">
         <f>AVERAGE(E3:E26)</f>
         <v>16.75</v>
       </c>
-      <c r="F28" s="108"/>
-      <c r="G28" s="109"/>
-      <c r="H28" s="96">
+      <c r="F28" s="71"/>
+      <c r="G28" s="72"/>
+      <c r="H28" s="67">
         <f>AVERAGE(H3:H26)</f>
         <v>6.833333333333333</v>
       </c>
-      <c r="I28" s="108"/>
-      <c r="J28" s="109"/>
-      <c r="K28" s="96">
+      <c r="I28" s="71"/>
+      <c r="J28" s="72"/>
+      <c r="K28" s="67">
         <f>AVERAGE(K3:K26)</f>
         <v>4.416666666666667</v>
       </c>
-      <c r="L28" s="108"/>
-      <c r="M28" s="109"/>
-      <c r="N28" s="96">
+      <c r="L28" s="71"/>
+      <c r="M28" s="72"/>
+      <c r="N28" s="67">
         <f>AVERAGE(N3:N26)</f>
         <v>5.791666666666667</v>
       </c>
-      <c r="O28" s="108"/>
-      <c r="P28" s="109"/>
-      <c r="Q28" s="96">
+      <c r="O28" s="71"/>
+      <c r="P28" s="72"/>
+      <c r="Q28" s="67">
         <f>AVERAGE(Q3:Q26)</f>
         <v>7.458333333333333</v>
       </c>
-      <c r="R28" s="108"/>
-      <c r="S28" s="109"/>
-      <c r="T28" s="96">
+      <c r="R28" s="71"/>
+      <c r="S28" s="72"/>
+      <c r="T28" s="67">
         <f>AVERAGE(T3:T26)</f>
         <v>6.583333333333333</v>
       </c>
-      <c r="U28" s="108"/>
-      <c r="V28" s="109"/>
-      <c r="W28" s="96">
+      <c r="U28" s="71"/>
+      <c r="V28" s="72"/>
+      <c r="W28" s="67">
         <f>AVERAGE(W3:W26)</f>
         <v>6.666666666666667</v>
       </c>
-      <c r="X28" s="109"/>
-      <c r="Y28" s="109"/>
-      <c r="Z28" s="95">
+      <c r="X28" s="72"/>
+      <c r="Y28" s="72"/>
+      <c r="Z28" s="66">
         <f>AVERAGE(Z3:Z26)</f>
         <v>8.5416666666666661</v>
       </c>
-      <c r="AA28" s="108"/>
-      <c r="AB28" s="109"/>
-      <c r="AC28" s="96">
+      <c r="AA28" s="71"/>
+      <c r="AB28" s="72"/>
+      <c r="AC28" s="67">
         <f>AVERAGE(AC3:AC26)</f>
         <v>8.0416666666666661</v>
       </c>
-      <c r="AD28" s="108"/>
-      <c r="AE28" s="109"/>
-      <c r="AF28" s="96">
+      <c r="AD28" s="71"/>
+      <c r="AE28" s="72"/>
+      <c r="AF28" s="67">
         <f>AVERAGE(AF3:AF26)</f>
         <v>8.2083333333333339</v>
       </c>
-      <c r="AG28" s="108"/>
-      <c r="AH28" s="109"/>
-      <c r="AI28" s="96">
+      <c r="AG28" s="71"/>
+      <c r="AH28" s="72"/>
+      <c r="AI28" s="67">
         <f>AVERAGE(AI3:AI26)</f>
         <v>7.458333333333333</v>
       </c>
-      <c r="AJ28" s="108"/>
-      <c r="AK28" s="109"/>
-      <c r="AL28" s="96">
+      <c r="AJ28" s="71"/>
+      <c r="AK28" s="72"/>
+      <c r="AL28" s="67">
         <f>AVERAGE(AL3:AL26)</f>
         <v>8.4583333333333339</v>
       </c>
-      <c r="AM28" s="108"/>
-      <c r="AN28" s="109"/>
-      <c r="AO28" s="96">
+      <c r="AM28" s="71"/>
+      <c r="AN28" s="72"/>
+      <c r="AO28" s="67">
         <f>AVERAGE(AO3:AO26)</f>
         <v>8.5416666666666661</v>
       </c>
-      <c r="AP28" s="37">
+      <c r="AP28" s="34">
         <f>AVERAGE(AP3:AP26)</f>
         <v>1.9166666666666667</v>
       </c>
-      <c r="AQ28" s="34">
-        <f t="shared" ref="AQ28:AU30" si="12">AVERAGE(AQ3:AQ26)</f>
+      <c r="AQ28" s="31">
+        <f t="shared" ref="AQ28:AU28" si="12">AVERAGE(AQ3:AQ26)</f>
         <v>2.1666666666666665</v>
       </c>
-      <c r="AR28" s="34">
+      <c r="AR28" s="31">
         <f t="shared" si="12"/>
         <v>2.75</v>
       </c>
-      <c r="AS28" s="34">
+      <c r="AS28" s="31">
         <f t="shared" si="12"/>
         <v>2.7083333333333335</v>
       </c>
-      <c r="AT28" s="119">
+      <c r="AT28" s="82">
         <f t="shared" si="12"/>
         <v>0.83333333333333337</v>
       </c>
-      <c r="AU28" s="120">
+      <c r="AU28" s="83">
         <f t="shared" si="12"/>
         <v>0.54166666666666663</v>
       </c>
-      <c r="AV28" s="37">
+      <c r="AV28" s="34">
         <f>AVERAGE(H28,K28,N28)</f>
         <v>5.6805555555555562</v>
       </c>
-      <c r="AW28" s="34">
+      <c r="AW28" s="31">
         <f>AVERAGE(Q28,T28,W28)</f>
         <v>6.9027777777777777</v>
       </c>
-      <c r="AX28" s="34">
+      <c r="AX28" s="31">
         <f>AVERAGE(Z28,AC28,AF28)</f>
         <v>8.2638888888888875</v>
       </c>
-      <c r="AY28" s="34">
+      <c r="AY28" s="31">
         <f>AVERAGE(AI28,AL28,AO28)</f>
         <v>8.1527777777777786</v>
       </c>
-      <c r="AZ28" s="119">
+      <c r="AZ28" s="82">
         <f>AX28-AV28</f>
         <v>2.5833333333333313</v>
       </c>
-      <c r="BA28" s="120">
+      <c r="BA28" s="83">
         <f>AY28-AW28</f>
         <v>1.2500000000000009</v>
       </c>
     </row>
-    <row r="29" spans="1:53" s="110" customFormat="1" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="90"/>
-      <c r="B29" s="91"/>
-      <c r="C29" s="94" t="s">
-        <v>105</v>
-      </c>
-      <c r="D29" s="114">
+    <row r="29" spans="1:53" s="73" customFormat="1" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="97"/>
+      <c r="B29" s="98"/>
+      <c r="C29" s="65" t="s">
+        <v>104</v>
+      </c>
+      <c r="D29" s="77">
         <f>AVERAGE(D3:D14)</f>
         <v>39.083333333333336</v>
       </c>
-      <c r="E29" s="115">
+      <c r="E29" s="78">
         <f>AVERAGE(E3:E14)</f>
         <v>15.583333333333334</v>
       </c>
-      <c r="F29" s="108"/>
-      <c r="G29" s="109"/>
-      <c r="H29" s="96">
+      <c r="F29" s="71"/>
+      <c r="G29" s="72"/>
+      <c r="H29" s="67">
         <f>AVERAGE(H3:H14)</f>
         <v>6.5</v>
       </c>
-      <c r="I29" s="108"/>
-      <c r="J29" s="109"/>
-      <c r="K29" s="96">
+      <c r="I29" s="71"/>
+      <c r="J29" s="72"/>
+      <c r="K29" s="67">
         <f>AVERAGE(K3:K14)</f>
         <v>4.583333333333333</v>
       </c>
-      <c r="L29" s="108"/>
-      <c r="M29" s="109"/>
-      <c r="N29" s="96">
+      <c r="L29" s="71"/>
+      <c r="M29" s="72"/>
+      <c r="N29" s="67">
         <f>AVERAGE(N3:N14)</f>
         <v>6.583333333333333</v>
       </c>
-      <c r="O29" s="108"/>
-      <c r="P29" s="109"/>
-      <c r="Q29" s="96">
+      <c r="O29" s="71"/>
+      <c r="P29" s="72"/>
+      <c r="Q29" s="67">
         <f>AVERAGE(Q3:Q14)</f>
         <v>7.5</v>
       </c>
-      <c r="R29" s="108"/>
-      <c r="S29" s="109"/>
-      <c r="T29" s="96">
+      <c r="R29" s="71"/>
+      <c r="S29" s="72"/>
+      <c r="T29" s="67">
         <f>AVERAGE(T3:T14)</f>
         <v>6.75</v>
       </c>
-      <c r="U29" s="108"/>
-      <c r="V29" s="109"/>
-      <c r="W29" s="96">
+      <c r="U29" s="71"/>
+      <c r="V29" s="72"/>
+      <c r="W29" s="67">
         <f>AVERAGE(W3:W14)</f>
         <v>7.25</v>
       </c>
-      <c r="X29" s="109"/>
-      <c r="Y29" s="109"/>
-      <c r="Z29" s="95">
+      <c r="X29" s="72"/>
+      <c r="Y29" s="72"/>
+      <c r="Z29" s="66">
         <f>AVERAGE(Z3:Z14)</f>
         <v>8.9166666666666661</v>
       </c>
-      <c r="AA29" s="108"/>
-      <c r="AB29" s="109"/>
-      <c r="AC29" s="96">
+      <c r="AA29" s="71"/>
+      <c r="AB29" s="72"/>
+      <c r="AC29" s="67">
         <f>AVERAGE(AC3:AC14)</f>
         <v>7.833333333333333</v>
       </c>
-      <c r="AD29" s="108"/>
-      <c r="AE29" s="109"/>
-      <c r="AF29" s="96">
+      <c r="AD29" s="71"/>
+      <c r="AE29" s="72"/>
+      <c r="AF29" s="67">
         <f>AVERAGE(AF3:AF14)</f>
         <v>8.5833333333333339</v>
       </c>
-      <c r="AG29" s="108"/>
-      <c r="AH29" s="109"/>
-      <c r="AI29" s="96">
+      <c r="AG29" s="71"/>
+      <c r="AH29" s="72"/>
+      <c r="AI29" s="67">
         <f>AVERAGE(AI3:AI14)</f>
         <v>8.6666666666666661</v>
       </c>
-      <c r="AJ29" s="108"/>
-      <c r="AK29" s="109"/>
-      <c r="AL29" s="96">
+      <c r="AJ29" s="71"/>
+      <c r="AK29" s="72"/>
+      <c r="AL29" s="67">
         <f>AVERAGE(AL3:AL14)</f>
         <v>8.8333333333333339</v>
       </c>
-      <c r="AM29" s="108"/>
-      <c r="AN29" s="109"/>
-      <c r="AO29" s="96">
+      <c r="AM29" s="71"/>
+      <c r="AN29" s="72"/>
+      <c r="AO29" s="67">
         <f>AVERAGE(AO3:AO14)</f>
         <v>9.25</v>
       </c>
-      <c r="AP29" s="108"/>
-      <c r="AQ29" s="109"/>
-      <c r="AR29" s="109"/>
-      <c r="AS29" s="109"/>
-      <c r="AT29" s="119">
+      <c r="AP29" s="71"/>
+      <c r="AQ29" s="72"/>
+      <c r="AR29" s="72"/>
+      <c r="AS29" s="72"/>
+      <c r="AT29" s="82">
         <f>AVERAGE(AT3:AT14)</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="AU29" s="120">
+      <c r="AU29" s="83">
         <f>AVERAGE(AU3:AU14)</f>
         <v>1</v>
       </c>
-      <c r="AV29" s="37">
+      <c r="AV29" s="34">
         <f t="shared" ref="AV29:AV30" si="13">AVERAGE(H29,K29,N29)</f>
         <v>5.8888888888888884</v>
       </c>
-      <c r="AW29" s="34">
+      <c r="AW29" s="31">
         <f t="shared" ref="AW29:AW30" si="14">AVERAGE(Q29,T29,W29)</f>
         <v>7.166666666666667</v>
       </c>
-      <c r="AX29" s="34">
+      <c r="AX29" s="31">
         <f t="shared" ref="AX29:AX30" si="15">AVERAGE(Z29,AC29,AF29)</f>
         <v>8.4444444444444446</v>
       </c>
-      <c r="AY29" s="34">
+      <c r="AY29" s="31">
         <f t="shared" ref="AY29:AY30" si="16">AVERAGE(AI29,AL29,AO29)</f>
         <v>8.9166666666666661</v>
       </c>
-      <c r="AZ29" s="119">
+      <c r="AZ29" s="82">
         <f t="shared" ref="AZ29:AZ30" si="17">AX29-AV29</f>
         <v>2.5555555555555562</v>
       </c>
-      <c r="BA29" s="120">
+      <c r="BA29" s="83">
         <f t="shared" ref="BA29:BA30" si="18">AY29-AW29</f>
         <v>1.7499999999999991</v>
       </c>
     </row>
-    <row r="30" spans="1:53" s="113" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="92"/>
-      <c r="B30" s="93"/>
-      <c r="C30" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="D30" s="116">
+    <row r="30" spans="1:53" s="76" customFormat="1" ht="22" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="99"/>
+      <c r="B30" s="100"/>
+      <c r="C30" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="D30" s="79">
         <f>AVERAGE(D15:D26)</f>
         <v>41.25</v>
       </c>
-      <c r="E30" s="32">
+      <c r="E30" s="29">
         <f>AVERAGE(E15:E26)</f>
         <v>17.916666666666668</v>
       </c>
-      <c r="F30" s="111"/>
-      <c r="G30" s="112"/>
+      <c r="F30" s="74"/>
+      <c r="G30" s="75"/>
       <c r="H30" s="27">
         <f>AVERAGE(H15:H26)</f>
         <v>7.166666666666667</v>
       </c>
-      <c r="I30" s="111"/>
-      <c r="J30" s="112"/>
+      <c r="I30" s="74"/>
+      <c r="J30" s="75"/>
       <c r="K30" s="27">
         <f>AVERAGE(K15:K26)</f>
         <v>4.25</v>
       </c>
-      <c r="L30" s="111"/>
-      <c r="M30" s="112"/>
+      <c r="L30" s="74"/>
+      <c r="M30" s="75"/>
       <c r="N30" s="27">
         <f>AVERAGE(N15:N26)</f>
         <v>5</v>
       </c>
-      <c r="O30" s="111"/>
-      <c r="P30" s="112"/>
+      <c r="O30" s="74"/>
+      <c r="P30" s="75"/>
       <c r="Q30" s="27">
         <f>AVERAGE(Q15:Q26)</f>
         <v>7.416666666666667</v>
       </c>
-      <c r="R30" s="111"/>
-      <c r="S30" s="112"/>
+      <c r="R30" s="74"/>
+      <c r="S30" s="75"/>
       <c r="T30" s="27">
         <f>AVERAGE(T15:T26)</f>
         <v>6.416666666666667</v>
       </c>
-      <c r="U30" s="111"/>
-      <c r="V30" s="112"/>
+      <c r="U30" s="74"/>
+      <c r="V30" s="75"/>
       <c r="W30" s="27">
         <f>AVERAGE(W15:W26)</f>
         <v>6.083333333333333</v>
       </c>
-      <c r="X30" s="112"/>
-      <c r="Y30" s="112"/>
-      <c r="Z30" s="32">
+      <c r="X30" s="75"/>
+      <c r="Y30" s="75"/>
+      <c r="Z30" s="29">
         <f>AVERAGE(Z15:Z26)</f>
         <v>8.1666666666666661</v>
       </c>
-      <c r="AA30" s="111"/>
-      <c r="AB30" s="112"/>
+      <c r="AA30" s="74"/>
+      <c r="AB30" s="75"/>
       <c r="AC30" s="27">
         <f>AVERAGE(AC15:AC26)</f>
         <v>8.25</v>
       </c>
-      <c r="AD30" s="111"/>
-      <c r="AE30" s="112"/>
+      <c r="AD30" s="74"/>
+      <c r="AE30" s="75"/>
       <c r="AF30" s="27">
         <f>AVERAGE(AF15:AF26)</f>
         <v>7.833333333333333</v>
       </c>
-      <c r="AG30" s="111"/>
-      <c r="AH30" s="112"/>
+      <c r="AG30" s="74"/>
+      <c r="AH30" s="75"/>
       <c r="AI30" s="27">
         <f>AVERAGE(AI15:AI26)</f>
         <v>6.25</v>
       </c>
-      <c r="AJ30" s="111"/>
-      <c r="AK30" s="112"/>
+      <c r="AJ30" s="74"/>
+      <c r="AK30" s="75"/>
       <c r="AL30" s="27">
         <f>AVERAGE(AL15:AL26)</f>
         <v>8.0833333333333339</v>
       </c>
-      <c r="AM30" s="111"/>
-      <c r="AN30" s="112"/>
+      <c r="AM30" s="74"/>
+      <c r="AN30" s="75"/>
       <c r="AO30" s="27">
         <f>AVERAGE(AO15:AO26)</f>
         <v>7.833333333333333</v>
       </c>
-      <c r="AP30" s="111"/>
-      <c r="AQ30" s="112"/>
-      <c r="AR30" s="112"/>
-      <c r="AS30" s="112"/>
-      <c r="AT30" s="121">
+      <c r="AP30" s="74"/>
+      <c r="AQ30" s="75"/>
+      <c r="AR30" s="75"/>
+      <c r="AS30" s="75"/>
+      <c r="AT30" s="84">
         <f>AVERAGE(AT15:AT26)</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="AU30" s="122">
+      <c r="AU30" s="85">
         <f>AVERAGE(AU15:AU26)</f>
         <v>8.3333333333333329E-2</v>
       </c>
@@ -14403,11 +13981,11 @@
         <f t="shared" si="16"/>
         <v>7.3888888888888893</v>
       </c>
-      <c r="AZ30" s="121">
+      <c r="AZ30" s="84">
         <f t="shared" si="17"/>
         <v>2.6111111111111098</v>
       </c>
-      <c r="BA30" s="122">
+      <c r="BA30" s="85">
         <f t="shared" si="18"/>
         <v>0.75</v>
       </c>
@@ -14415,65 +13993,97 @@
     <row r="31" spans="1:53" x14ac:dyDescent="0.2">
       <c r="B31"/>
       <c r="C31"/>
-      <c r="AT31" s="97"/>
-      <c r="AU31" s="97"/>
+      <c r="AT31" s="68"/>
+      <c r="AU31" s="68"/>
     </row>
     <row r="32" spans="1:53" ht="22" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B32"/>
       <c r="C32"/>
-      <c r="AT32" s="98"/>
-      <c r="AU32" s="98"/>
+      <c r="D32"/>
+      <c r="G32"/>
+      <c r="H32"/>
+      <c r="I32"/>
+      <c r="AH32"/>
+      <c r="AI32"/>
+      <c r="AT32" s="68"/>
+      <c r="AU32" s="68"/>
     </row>
     <row r="33" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A33" s="126" t="s">
+      <c r="A33" s="122" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="123" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" s="124" t="s">
+        <v>74</v>
+      </c>
+      <c r="D33"/>
+      <c r="G33"/>
+      <c r="H33"/>
+      <c r="I33"/>
+      <c r="AH33"/>
+      <c r="AI33"/>
+      <c r="AT33" s="101" t="s">
+        <v>76</v>
+      </c>
+      <c r="AU33" s="102"/>
+    </row>
+    <row r="34" spans="1:47" ht="22" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="125" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" s="126" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" s="127" t="s">
         <v>75</v>
       </c>
-      <c r="B33" s="126"/>
-      <c r="C33" s="127" t="s">
-        <v>64</v>
-      </c>
-      <c r="D33" s="127" t="s">
-        <v>37</v>
-      </c>
-      <c r="AT33" s="102" t="s">
-        <v>77</v>
-      </c>
-      <c r="AU33" s="103"/>
-    </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A34" s="62" t="s">
-        <v>76</v>
-      </c>
-      <c r="B34" s="62"/>
-      <c r="C34" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="D34" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="G34" s="31"/>
-      <c r="H34" s="31"/>
-      <c r="AT34" s="104"/>
-      <c r="AU34" s="105"/>
+      <c r="D34"/>
+      <c r="G34"/>
+      <c r="H34"/>
+      <c r="I34"/>
+      <c r="AH34"/>
+      <c r="AI34"/>
+      <c r="AT34" s="103"/>
+      <c r="AU34" s="104"/>
     </row>
     <row r="35" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="AT35" s="104"/>
-      <c r="AU35" s="105"/>
+      <c r="D35"/>
+      <c r="G35"/>
+      <c r="H35"/>
+      <c r="I35"/>
+      <c r="AH35"/>
+      <c r="AI35"/>
+      <c r="AT35" s="103"/>
+      <c r="AU35" s="104"/>
     </row>
     <row r="36" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="AT36" s="104"/>
-      <c r="AU36" s="105"/>
+      <c r="D36"/>
+      <c r="G36"/>
+      <c r="H36"/>
+      <c r="I36"/>
+      <c r="AH36"/>
+      <c r="AI36"/>
+      <c r="AT36" s="103"/>
+      <c r="AU36" s="104"/>
     </row>
     <row r="37" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="AT37" s="104"/>
-      <c r="AU37" s="105"/>
+      <c r="G37"/>
+      <c r="H37"/>
+      <c r="I37"/>
+      <c r="AT37" s="103"/>
+      <c r="AU37" s="104"/>
     </row>
     <row r="38" spans="1:47" ht="22" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AT38" s="106"/>
-      <c r="AU38" s="107"/>
+      <c r="G38"/>
+      <c r="H38"/>
+      <c r="I38"/>
+      <c r="AT38" s="105"/>
+      <c r="AU38" s="106"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="10">
     <mergeCell ref="AP1:AU1"/>
     <mergeCell ref="AV1:BA1"/>
     <mergeCell ref="A27:B30"/>
@@ -14484,8 +14094,6 @@
     <mergeCell ref="O1:W1"/>
     <mergeCell ref="X1:AF1"/>
     <mergeCell ref="AG1:AO1"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="AT3:AU26 AZ3:BA27">
@@ -14501,13 +14109,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT3:AU26 AZ3:BA26">
-    <cfRule type="cellIs" dxfId="44" priority="18" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="18" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="19" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="20" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>